<commit_message>
Pass simulation Test Plan. Add ILAs. Ready to generate bitstream.
</commit_message>
<xml_diff>
--- a/docs/Test Plan y Mapa de Registros.xlsx
+++ b/docs/Test Plan y Mapa de Registros.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajmsalgado\SynologyDrive\Universidad\TFM\pwm_enjoyer\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF5251B-BFD0-4F1C-AC3C-D5FE21F97DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA2CF30-A908-4425-9E1D-4248A08EACEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="196">
   <si>
     <t>Nombre</t>
   </si>
@@ -165,9 +165,6 @@
     <t>Funcionamiento correcto.</t>
   </si>
   <si>
-    <t>Funcionamiento erróneo e imprevisible.</t>
-  </si>
-  <si>
     <t>11.1</t>
   </si>
   <si>
@@ -210,9 +207,6 @@
     <t>Procedimiento normal</t>
   </si>
   <si>
-    <t>Pulso activo en la señal de reset.</t>
-  </si>
-  <si>
     <t>Todos los módulos se quedan a '0'. Las memorias no pierden sus configuraciones guardadas.</t>
   </si>
   <si>
@@ -249,9 +243,6 @@
     <t>Selector del PWM_0</t>
   </si>
   <si>
-    <t>0: -                                                     1: Selec.</t>
-  </si>
-  <si>
     <t>Selecciona los módulos a configurar. Tantos registros de este estilo como número de PWMs % 32.</t>
   </si>
   <si>
@@ -279,9 +270,6 @@
     <t>Apaga todo, reset global</t>
   </si>
   <si>
-    <t>0: -                                             1: Aplicar</t>
-  </si>
-  <si>
     <t>Sólo debe haber un bit activado. Último registro en activar tras los de configuración.</t>
   </si>
   <si>
@@ -339,9 +327,6 @@
     <t>Validación de escritura de WR_DATA</t>
   </si>
   <si>
-    <t>0: -                                            1: Enable</t>
-  </si>
-  <si>
     <t>Por cada estado configurado, se tiene que poner primero a '1' y luego a '0'.</t>
   </si>
   <si>
@@ -384,9 +369,6 @@
     <t>Indicador de redundancia en el PWM_0</t>
   </si>
   <si>
-    <t>0: OK                                       1: Error</t>
-  </si>
-  <si>
     <t>RED_31</t>
   </si>
   <si>
@@ -405,9 +387,6 @@
     <t>Error en la programación del PWM_0</t>
   </si>
   <si>
-    <t>0: OK                                      1: Error</t>
-  </si>
-  <si>
     <t>Aplica las configuraciones de los demás registros sobre los PWM seleccionados en este. Tantos registros de este estilo como número de PWMs % 32.</t>
   </si>
   <si>
@@ -426,18 +405,9 @@
     <t>Estado del IP</t>
   </si>
   <si>
-    <t>00: Apagados                01: Configurando                  10: Activos                   11: Error</t>
-  </si>
-  <si>
     <t>31:2</t>
   </si>
   <si>
-    <t>Se aplica la configuración previa. La nueva configuración se guarda en la memoria.</t>
-  </si>
-  <si>
-    <t>Se aplica la configuración previa. La nueva configuración se pierde ya que el IP está protegido ante este caso.</t>
-  </si>
-  <si>
     <t>TBD</t>
   </si>
   <si>
@@ -489,19 +459,95 @@
     <t>24</t>
   </si>
   <si>
+    <t>Puesta en marcha de un único PWM con los parámetros de configuración límites más bajos posibles. Apagar al final.</t>
+  </si>
+  <si>
+    <t>Puesta en marcha de un único PWM con parámetros de configuración por debajo de los límites inferiores. Apagar al final.</t>
+  </si>
+  <si>
+    <t>Valores por encima de máximos: supera N_ADDR</t>
+  </si>
+  <si>
+    <t>Puesta en marcha de un único PWM con parámetros de configuración por encima de los límites superiores respecto a N_ADDR (no tiene sentido intentar sumar por encima de FFFF_FFFF en N_TOT_CYC). Apagar al final.</t>
+  </si>
+  <si>
+    <t>Solución</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>Puesta en marcha de un único PWM con parámetros de configuración dentro de los rangos establecidos, siguiendo el orden de escritura en registros esperado. Una configuración. Apagar al final.</t>
+  </si>
+  <si>
+    <t>Puesta en marcha de un único PWM con parámetros de configuración dentro de los rangos establecidos, siguiendo el orden de escritura en registros esperado.Varias configuraciones. Apagar al final.</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Protegido. No debe entrar la configuración. Levanta error.</t>
+  </si>
+  <si>
     <t xml:space="preserve">1. Los datos se escriben mal en la memoria porque WR_EN solo consideraba entrada de WR_ADDR y WR_DATA durante un único flanco activo.
+2. WR_DATA_VALID no se resetea a la entrada de cada PWM (no actúa como un único pulso).
 </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">1. Se modifican STATE_CTRLR y PWM_DP_MEM para segmentar WR_EN y poder leer datos en diferentes transacciones AXI.
+    <t>1. Al poner los genéricos máximos nos damos cuenta de que hay un registro de 2^32 - 1 bits en STATE_CTRLR.
+2. Al llegar a la última dirección salta error.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Se modifican STATE_CTRLR y PWM_DP_MEM para segmentar WR_EN y poder leer datos en diferentes transacciones AXI.
+2. Se cambia la lógica del reset del registro a PWM_ENJOYER_AXI en lugar de en CONTROL_UNIT.
 </t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>Puesta en marcha de un único PWM con los parámetros de configuración límites en N_ADDR. Apagar al final.</t>
+  </si>
+  <si>
+    <t>Puesta en marcha de un único PWM con los parámetros de configuración límites en N_TOT_CYC. Apagar al final.</t>
+  </si>
+  <si>
+    <t>1. Se modifica PWM_DP_MEM, STATE_CTRLR y PWM_COUNTER para poder predecir un ciclo más del siguiente estado.
+2. Se cambia el valor del genérico G_MEM_SIZE_MAX_L2 a log2(G_MEM_SIZE_MAX_N + 1)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Funcionamiento correcto.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Requiere una simulación de 35 segundos, demasiado para el simulador de Vivado.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Configuración del PWM_0, 4 estados: (1,5,3,1), empezando a nivel alto:</t>
     </r>
     <r>
       <rPr>
@@ -512,59 +558,24 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <t>1. Al poner los genéricos máximos nos damos cuenta de que hay un registro de 2^32 - 1 bits en STATE_CTRLR.</t>
-  </si>
-  <si>
-    <t>1. Se modifica PWM_DP_MEM, STATE_CTRLR y PWM_COUNTER para poder predecir un ciclo más del siguiente estado.</t>
-  </si>
-  <si>
-    <t>Puesta en marcha de un único PWM con parámetros de configuración dentro de los rangos establecidos, siguiendo el orden de escritura en registros esperado. Apagar al final.</t>
-  </si>
-  <si>
-    <t>Puesta en marcha de un único PWM con los parámetros de configuración límites más bajos posibles. Apagar al final.</t>
-  </si>
-  <si>
-    <t>Puesta en marcha de un único PWM con parámetros de configuración por debajo de los límites inferiores. Apagar al final.</t>
-  </si>
-  <si>
-    <t>4.1</t>
-  </si>
-  <si>
-    <t>Puesta en marcha de un único PWM con los parámetros de configuración límites más altos posibles. Apagar al final.
-- 128 estados
-- Cada uno de ellos de valor 01FF_FFFF</t>
-  </si>
-  <si>
-    <t>Valores por encima de máximos: supera N_ADDR</t>
-  </si>
-  <si>
-    <t>Puesta en marcha de un único PWM con parámetros de configuración por encima de los límites superiores respecto a N_ADDR (no tiene sentido intentar sumar por encima de FFFF_FFFF en N_TOT_CYC). Apagar al final.</t>
-  </si>
-  <si>
-    <t>Configuración del PWM_0, 4 estados: (1,5,3,1), empezando nivel alto:
-&gt;&gt; REG_DIRECCIONES(0x00)= 0x00000001
+&gt;&gt; REG_DIRECCIONES(0x00) = 0x00000001
 &gt;&gt; REG_CONTROL(0x04) = 0x00000008
 &gt;&gt; REG_N_ADDR(0x10) = 0x00000004
 &gt;&gt; REG_N_TOT_CYC(0x14) = 0x0000000A
 &gt;&gt; REG_PWM_INIT(0x18) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x00000001
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x00000005
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x00000003
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x00000001
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
-wait 2 clk_period
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
+wait clk_period
 &gt;&gt; REG_CONTROL(0x04) = 0x00000004
 wait 1 min
-reset = '1'</t>
-  </si>
-  <si>
+</t>
+    </r>
     <r>
       <rPr>
         <i/>
@@ -574,7 +585,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Configuración del PWM_0, 4 estados: (1,5,3,1), empezando nivel alto:</t>
+      <t>Apagado:</t>
     </r>
     <r>
       <rPr>
@@ -585,23 +596,7 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-&gt;&gt; REG_DIRECCIONES(0x00)= 0x00000001
-&gt;&gt; REG_CONTROL(0x04) = 0x00000008
-&gt;&gt; REG_N_ADDR(0x10) = 0x00000004
-&gt;&gt; REG_N_TOT_CYC(0x14) = 0x0000000A
-&gt;&gt; REG_PWM_INIT(0x18) = 0x00000001
-&gt;&gt; REG_WR_DATA(0x08) = 0x00000001
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
-&gt;&gt; REG_WR_DATA(0x08) = 0x00000005
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
-&gt;&gt; REG_WR_DATA(0x08) = 0x00000003
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
-&gt;&gt; REG_WR_DATA(0x08) = 0x00000001
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
-wait 2 clk_period
-&gt;&gt; REG_CONTROL(0x04) = 0x00000004
-wait 1 min
-&gt;&gt; REG_DIRECCIONES(0x00)= 0x00000001
+&gt;&gt; REG_DIRECCIONES(0x00) = 0x00000001
 &gt;&gt; REG_CONTROL(0x04) = 0x00000002</t>
     </r>
   </si>
@@ -615,7 +610,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Configuración del PWM_0, 2 estados (1,1), empezando nivel alto:</t>
+      <t>Configuración del PWM_0, 2 estados (1,1), empezando a nivel alto:</t>
     </r>
     <r>
       <rPr>
@@ -626,19 +621,41 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-&gt;&gt; REG_DIRECCIONES(0x00)= 0x00000001
+&gt;&gt; REG_DIRECCIONES(0x00) = 0x00000001
 &gt;&gt; REG_CONTROL(0x04) = 0x00000008
 &gt;&gt; REG_N_ADDR(0x10) = 0x00000002
 &gt;&gt; REG_N_TOT_CYC(0x14) = 0x00000002
 &gt;&gt; REG_PWM_INIT(0x18) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x00000001
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x00000001
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
-wait 2 clk_period
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
+wait clk_period
 &gt;&gt; REG_CONTROL(0x04) = 0x00000004
 wait 1 min
-&gt;&gt; REG_DIRECCIONES(0x00)= 0x00000001
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Apagado:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+&gt;&gt; REG_DIRECCIONES(0x00) = 0x00000001
 &gt;&gt; REG_CONTROL(0x04) = 0x00000002</t>
     </r>
   </si>
@@ -652,7 +669,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Configuración del PWM_0, 1 estado (1), empezando nivel alto:</t>
+      <t>Configuración del PWM_0, 1 estado (1), empezando a nivel alto:</t>
     </r>
     <r>
       <rPr>
@@ -663,17 +680,157 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-&gt;&gt; REG_DIRECCIONES(0x00)= 0x00000001
+&gt;&gt; REG_DIRECCIONES(0x00) = 0x00000001
+&gt;&gt; REG_CONTROL(0x04) = 0x00000008
+&gt;&gt; REG_N_ADDR(0x10) = 0x00000001
+&gt;&gt; REG_N_TOT_CYC(0x14) = 0x00000001
+&gt;&gt; REG_PWM_INIT(0x18) = 0x00000001
+&gt;&gt; REG_WR_DATA(0x08) = 0x00000001
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
+wait clk_period
+&gt;&gt; REG_CONTROL(0x04) = 0x00000004
+wait 1 min
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Apagado:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+&gt;&gt; REG_DIRECCIONES(0x00 ) = 0x00000001
+&gt;&gt; REG_CONTROL(0x04) = 0x00000002</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Configuración del PWM_0, 128 estados (todos desde el 1 hasta el 128), empezando a nivel alto:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+&gt;&gt; REG_DIRECCIONES(0x00) = 0x00000001
+&gt;&gt; REG_CONTROL(0x04) = 0x00000008
+&gt;&gt; REG_N_ADDR(0x10) = 0x00000080
+&gt;&gt; REG_N_TOT_CYC(0x14) = 0x00002040
+&gt;&gt; REG_PWM_INIT(0x18) = 0x00000001
+128 iteraciones, incrementando i {
+    &gt;&gt; REG_WR_DATA(0x08) = 0x00000001 + i
+    &gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
+}
+wait clk_period
+&gt;&gt; REG_CONTROL(0x04) = 0x00000004
+wait 1 min
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Apagado:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+&gt;&gt; REG_DIRECCIONES(0x00 ) = 0x00000001
+&gt;&gt; REG_CONTROL(0x04) = 0x00000002</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Configuración del PWM_0, 2 estados (FFFF_0000, 0000_FFFF), empezando a nivel alto:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+&gt;&gt; REG_DIRECCIONES(0x00) = 0x00000001
 &gt;&gt; REG_CONTROL(0x04) = 0x00000008
 &gt;&gt; REG_N_ADDR(0x10) = 0x00000002
-&gt;&gt; REG_N_TOT_CYC(0x14) = 0x00000002
+&gt;&gt; REG_N_TOT_CYC(0x14) = 0xFFFFFFFF
 &gt;&gt; REG_PWM_INIT(0x18) = 0x00000001
-&gt;&gt; REG_WR_DATA(0x08) = 0x00000001
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
-wait 2 clk_period
+&gt;&gt; REG_WR_DATA(0x08) = 0xFFFF0000
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
+&gt;&gt; REG_WR_DATA(0x08) = 0x0000FFFF
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
+wait clk_period
 &gt;&gt; REG_CONTROL(0x04) = 0x00000004
 wait 1 min
-&gt;&gt; REG_DIRECCIONES(0x00)= 0x00000001
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Apagado:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+&gt;&gt; REG_DIRECCIONES(0x00 ) = 0x00000001
 &gt;&gt; REG_CONTROL(0x04) = 0x00000002</t>
     </r>
   </si>
@@ -687,7 +844,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Configuración del PWM_0, 128 estados (todos 01FF_FFFF), empezando nivel alto:</t>
+      <t>Configuración del PWM_0, 129 estados (desde el 1 hasta el 129), empezando a nivel alto:</t>
     </r>
     <r>
       <rPr>
@@ -698,56 +855,41 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-&gt;&gt; REG_DIRECCIONES(0x00)= 0x00000001
+&gt;&gt; REG_DIRECCIONES(0x00) = 0x00000001
 &gt;&gt; REG_CONTROL(0x04) = 0x00000008
-&gt;&gt; REG_N_ADDR(0x10) = 0x00000080
-&gt;&gt; REG_N_TOT_CYC(0x14) = 0xFFFFFF80
-&gt;&gt; REG_PWM_INIT(0x18) = 0x00000001
-repetir 128 veces {
-    &gt;&gt; REG_WR_DATA(0x08) = 0x01FFFFFF
-    &gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
-}
-wait 2 clk_period
-&gt;&gt; REG_CONTROL(0x04) = 0x00000004
-wait 1 min
-&gt;&gt; REG_DIRECCIONES(0x00)= 0x00000001
-&gt;&gt; REG_CONTROL(0x04) = 0x00000002</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Configuración del PWM_0, 129 estados (desde el 1 hasta el 129), empezando nivel alto:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-&gt;&gt; REG_DIRECCIONES(0x00)= 0x00000001
-&gt;&gt; REG_CONTROL(0x04) = 0x00000008
-&gt;&gt; REG_N_ADDR(0x10) = 0x00000080
-&gt;&gt; REG_N_TOT_CYC(0x14) = 0xFFFFFF80
+&gt;&gt; REG_N_ADDR(0x10) = 0x00000081
+&gt;&gt; REG_N_TOT_CYC(0x14) = 0x000020C1
 &gt;&gt; REG_PWM_INIT(0x18) = 0x00000001
 129 iteraciones, incrementando i {
     &gt;&gt; REG_WR_DATA(0x08) = 0x00000001 + i
-    &gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+    &gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
 }
-wait 2 clk_period
+wait clk_period
 &gt;&gt; REG_CONTROL(0x04) = 0x00000004
 wait 1 min
-&gt;&gt; REG_DIRECCIONES(0x00)= 0x00000001
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Apagado:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+&gt;&gt; REG_DIRECCIONES(0x00) = 0x00000001
 &gt;&gt; REG_CONTROL(0x04) = 0x00000002</t>
     </r>
   </si>
@@ -772,26 +914,69 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-&gt;&gt; REG_DIRECCIONES(0x00)= 0x00000003
+&gt;&gt; REG_DIRECCIONES(0x00) = 0x00000007
 &gt;&gt; REG_CONTROL(0x04) = 0x00000008
 &gt;&gt; REG_N_ADDR(0x10) = 0x00000064
 &gt;&gt; REG_N_TOT_CYC(0x14) = 0x000013BA
 &gt;&gt; REG_PWM_INIT(0x18) = 0x00000000
 100 iteraciones, decrementando i {
-    &gt;&gt; REG_WR_DATA(0x08) = 0x00000064 - i
-    &gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+    &gt;&gt; REG_WR_DATA(0x08) = 0x0000000 + i
+    &gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
 }
-wait 2 clk_period
+wait clk_period
 &gt;&gt; REG_CONTROL(0x04) = 0x00000004
 wait 1 min
-&gt;&gt; REG_DIRECCIONES(0x00)= 0x00000003
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Apagado:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+&gt;&gt; REG_DIRECCIONES(0x00) = 0x00000007
 &gt;&gt; REG_CONTROL(0x04) = 0x00000002</t>
     </r>
   </si>
   <si>
+    <t>No deja correr la simulación, ya que excede el valor del genérico de BRAM_DUALPORT. En todo caso, debería estar protegido, no dejando entrar la configuración y levantando el error.</t>
+  </si>
+  <si>
+    <t>1. Si el anterior es es el Test 3 (levanta error) no aplica la nueva configuración.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Modificado CONTROL_UNIT y PWM_DP_MEM para evitar cargar configuraciones cuando N_ADDR &lt; 2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>VERIFICAR EN WAVEFORMS.</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Repetir 4 veces (i desde 0 hasta 3) {
-   </t>
+    </t>
     </r>
     <r>
       <rPr>
@@ -802,36 +987,58 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Configuración del PWM_i, 4 estados: (1,5,3,1), empezando nivel bajo:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-    &gt;&gt; REG_DIRECCIONES(0x00)= 0x00000001 * 2i
+      <t xml:space="preserve">Configuración del PWM_i, 4 estados: (1,5,3,1), empezando a nivel alto:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">    &gt;&gt; REG_DIRECCIONES(0x00) = 0x00000000 + 2^i
     &gt;&gt; REG_CONTROL(0x04) = 0x00000008
     &gt;&gt; REG_N_ADDR(0x10) = 0x00000004
     &gt;&gt; REG_N_TOT_CYC(0x14) = 0x0000000A
     &gt;&gt; REG_PWM_INIT(0x18) = 0x00000001
     &gt;&gt; REG_WR_DATA(0x08) = 0x00000001
-    &gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+    &gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
     &gt;&gt; REG_WR_DATA(0x08) = 0x00000005
-    &gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+    &gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
     &gt;&gt; REG_WR_DATA(0x08) = 0x00000003
-    &gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+    &gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
     &gt;&gt; REG_WR_DATA(0x08) = 0x00000001
-    &gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
-    wait 2 clk_period
+    &gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
+    wait clk_period
     &gt;&gt; REG_CONTROL(0x04) = 0x00000004
 }
 wait 1 min
 Repetir 4 veces (i desde 0 hasta 3) {
-    &gt;&gt; REG_DIRECCIONES(0x00)= 0x00000001 * 2i
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Apagado:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    &gt;&gt; REG_DIRECCIONES(0x00) = 0x00000000 + 2^i
     &gt;&gt; REG_CONTROL(0x04) = 0x00000002
 }</t>
     </r>
@@ -850,7 +1057,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Configuración del PWM_i, 4 estados: (1,5,3,1), empezando nivel bajo:</t>
+      <t>Configuración del PWM_i, 4 estados: (1,5,3,1), empezando a nivel alto:</t>
     </r>
     <r>
       <rPr>
@@ -861,23 +1068,45 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-    &gt;&gt; REG_DIRECCIONES(0x00)= 0x00000001 * 2i
+    &gt;&gt; REG_DIRECCIONES(0x00) = 0x00000000 + 2^i
     &gt;&gt; REG_CONTROL(0x04) = 0x00000008
     &gt;&gt; REG_N_ADDR(0x10) = 0x00000004
     &gt;&gt; REG_N_TOT_CYC(0x14) = 0x0000000A
     &gt;&gt; REG_PWM_INIT(0x18) = 0x00000001
     &gt;&gt; REG_WR_DATA(0x08) = 0x00000001
-    &gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+    &gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
     &gt;&gt; REG_WR_DATA(0x08) = 0x00000005
-    &gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+    &gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
     &gt;&gt; REG_WR_DATA(0x08) = 0x00000003
-    &gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+    &gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
     &gt;&gt; REG_WR_DATA(0x08) = 0x00000001
-    &gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
-    wait 2 clk_period
+    &gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
+    wait clk_period
     &gt;&gt; REG_CONTROL(0x04) = 0x00000004
 }
 wait 1 min
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Shutdown:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 &gt;&gt; REG_CONTROL(0x04) = 0x00000001</t>
     </r>
   </si>
@@ -891,7 +1120,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Configuración del PWM_0, 3 estados: (1,5,3) empezando nivel alto, aunque se esperan 4:</t>
+      <t>Configuración del PWM_0, 3 estados: (1,5,3) empezando a nivel alto, aunque se esperan 4:</t>
     </r>
     <r>
       <rPr>
@@ -902,18 +1131,18 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-&gt;&gt; REG_DIRECCIONES(0x00)= 0x00000001
+&gt;&gt; REG_DIRECCIONES(0x00) = 0x00000001
 &gt;&gt; REG_CONTROL(0x04) = 0x00000008
 &gt;&gt; REG_N_ADDR(0x10) = 0x00000004
 &gt;&gt; REG_N_TOT_CYC(0x14) = 0x00000009
 &gt;&gt; REG_PWM_INIT(0x18) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x00000001
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x00000005
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x00000003
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
-wait 2 clk_period
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
+wait clk_period
 &gt;&gt; REG_CONTROL(0x04) = 0x00000004</t>
     </r>
   </si>
@@ -927,7 +1156,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Configuración del PWM_0, 5 estados: (1,5,3,3,1) empezando nivel alto, aunque se esperan 4:</t>
+      <t>Configuración del PWM_0, 5 estados: (1,5,3,3,1) empezando a nivel alto, aunque se esperan 4:</t>
     </r>
     <r>
       <rPr>
@@ -938,22 +1167,22 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-&gt;&gt; REG_DIRECCIONES(0x00)= 0x00000001
+&gt;&gt; REG_DIRECCIONES(0x00) = 0x00000001
 &gt;&gt; REG_CONTROL(0x04) = 0x00000008
 &gt;&gt; REG_N_ADDR(0x10) = 0x00000004
 &gt;&gt; REG_N_TOT_CYC(0x14) = 0x0000000D
 &gt;&gt; REG_PWM_INIT(0x18) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x00000001
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x00000005
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x00000003
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x00000003
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x00000001
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
-wait 2 clk_period
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
+wait clk_period
 &gt;&gt; REG_CONTROL(0x04) = 0x00000004</t>
     </r>
   </si>
@@ -967,7 +1196,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Configuración del PWM_0, 4 estados: (1,5,3,1), empezando nivel alto:</t>
+      <t>Configuración del PWM_0, 4 estados: (1,5,3,1), empezando a nivel alto. Suma escrita = 11:</t>
     </r>
     <r>
       <rPr>
@@ -978,20 +1207,20 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-&gt;&gt; REG_DIRECCIONES(0x00)= 0x00000001
+&gt;&gt; REG_DIRECCIONES(0x00) = 0x00000001
 &gt;&gt; REG_CONTROL(0x04) = 0x00000008
 &gt;&gt; REG_N_ADDR(0x10) = 0x00000004
 &gt;&gt; REG_N_TOT_CYC(0x14) = 0x0000000B
 &gt;&gt; REG_PWM_INIT(0x18) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x00000001
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x00000005
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x00000003
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x00000001
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
-wait 2 clk_period
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
+wait clk_period
 &gt;&gt; REG_CONTROL(0x04) = 0x00000004</t>
     </r>
   </si>
@@ -1005,7 +1234,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Configuración del PWM_0, 4 estados: (1,5,3,1), empezando nivel alto:</t>
+      <t>Configuración del PWM_0, 4 estados: (1,5,3,1), empezando a nivel alto. Suma escrita = 9:</t>
     </r>
     <r>
       <rPr>
@@ -1016,27 +1245,24 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-&gt;&gt; REG_DIRECCIONES(0x00)= 0x00000001
+&gt;&gt; REG_DIRECCIONES(0x00) = 0x00000001
 &gt;&gt; REG_CONTROL(0x04) = 0x00000008
 &gt;&gt; REG_N_ADDR(0x10) = 0x00000004
 &gt;&gt; REG_N_TOT_CYC(0x14) = 0x00000009
 &gt;&gt; REG_PWM_INIT(0x18) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x00000001
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x00000005
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x00000003
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x00000001
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
-wait 2 clk_period
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
+wait clk_period
 &gt;&gt; REG_CONTROL(0x04) = 0x00000004</t>
     </r>
   </si>
   <si>
-    <t>Solución</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <i/>
@@ -1046,7 +1272,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Primera configuración del PWM_0, 4 estados: (1,5,3,1), empezando nivel alto:</t>
+      <t>Primera configuración del PWM_0, 4 estados: (1,5,3,1), empezando a nivel alto:</t>
     </r>
     <r>
       <rPr>
@@ -1057,6 +1283,7 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
+&gt;&gt; Mismas instrucciones que el Test 1 hasta el apagado
 </t>
     </r>
     <r>
@@ -1068,7 +1295,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>&gt;&gt; Mismas instrucciones que el Test 1 hasta el apagado</t>
+      <t>Update anticipado</t>
     </r>
     <r>
       <rPr>
@@ -1079,26 +1306,45 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-Segunda configuración del PWM_0, 3 estados: (10,20,15), empezando nivel alto:
-&gt;&gt; REG_DIRECCIONES(0x00)= 0x00000001
+&gt;&gt; REG_CONTROL(0x04) = 0x00000004
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Segunda configuración del PWM_0, 3 estados: (10,20,15), empezando a nivel alto:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&gt;&gt; REG_DIRECCIONES(0x00) = 0x00000001
 &gt;&gt; REG_CONTROL(0x04) = 0x00000008
 &gt;&gt; REG_N_ADDR(0x10) = 0x00000003
 &gt;&gt; REG_N_TOT_CYC(0x14) = 0x0000002D
 &gt;&gt; REG_PWM_INIT(0x18) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x0000000A
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x00000014
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
-Update anticipado:
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
+&gt;&gt; REG_WR_DATA(0x08) = 0x0000000F
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
+wait clk_period
 &gt;&gt; REG_CONTROL(0x04) = 0x00000004
-&gt;&gt; REG_WR_DATA(0x08) = 0x0000000F
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
-wait 2 clk_period
-&gt;&gt; REG_CONTROL(0x04) = 0x00000004
-wait 1 min</t>
-    </r>
-  </si>
-  <si>
+wait 1 min
+</t>
+    </r>
     <r>
       <rPr>
         <i/>
@@ -1108,7 +1354,32 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Primera configuración del PWM_0, 4 estados: (1,5,3,1), empezando nivel alto:</t>
+      <t>Apagado</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:
+&gt;&gt; REG_DIRECCIONES(0x00) = 0x00000001
+&gt;&gt; REG_CONTROL(0x04) = 0x00000002</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Primera configuración del PWM_0, 4 estados: (1,5,3,1), empezando a nivel alto:</t>
     </r>
     <r>
       <rPr>
@@ -1119,6 +1390,7 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
+&gt;&gt; Mismas instrucciones que el Test 1 hasta el apagado
 </t>
     </r>
     <r>
@@ -1130,7 +1402,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>&gt;&gt; Mismas instrucciones que el Test 1 hasta el apagado</t>
+      <t>Segunda configuración del PWM_0, 3 estados: (10,20,15), empezando a nivel alto:</t>
     </r>
     <r>
       <rPr>
@@ -1141,68 +1413,24 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Update anticipado</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-&gt;&gt; REG_CONTROL(0x04) = 0x00000004
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Segunda configuración del PWM_0, 3 estados: (10,20,15), empezando nivel alto:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&gt;&gt; REG_DIRECCIONES(0x00)= 0x00000001
+&gt;&gt; REG_DIRECCIONES(0x00) = 0x00000001
 &gt;&gt; REG_CONTROL(0x04) = 0x00000008
 &gt;&gt; REG_N_ADDR(0x10) = 0x00000003
 &gt;&gt; REG_N_TOT_CYC(0x14) = 0x0000002D
 &gt;&gt; REG_PWM_INIT(0x18) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x0000000A
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x00000014
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
+Update anticipado:
+&gt;&gt; REG_CONTROL(0x04) = 0x00000004
 &gt;&gt; REG_WR_DATA(0x08) = 0x0000000F
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
-wait 2 clk_period
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
+wait clk_period
 &gt;&gt; REG_CONTROL(0x04) = 0x00000004
-wait 1 min</t>
-    </r>
-  </si>
-  <si>
+wait 1 min
+</t>
+    </r>
     <r>
       <rPr>
         <i/>
@@ -1212,21 +1440,25 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Primera configuración del PWM_0, 4 estados: (1,5,3,1), empezando nivel alto:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">
+Apagado:
 </t>
     </r>
     <r>
       <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;&gt; REG_DIRECCIONES(0x00) = 0x00000001
+&gt;&gt; REG_CONTROL(0x04) = 0x00000002</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
         <i/>
         <sz val="11"/>
         <color theme="1"/>
@@ -1234,7 +1466,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>&gt;&gt; Mismas instrucciones que el Test 1 hasta el apagado</t>
+      <t>Primera configuración del PWM_0, 4 estados: (1,5,3,1), empezando a nivel alto:</t>
     </r>
     <r>
       <rPr>
@@ -1245,59 +1477,435 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-Segunda configuración del PWM_0, 3 estados: (10,20,15), empezando nivel alto:
-&gt;&gt; REG_DIRECCIONES(0x00)= 0x00000001
+&gt;&gt; Mismas instrucciones que el Test 1 hasta el apagado
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Segunda configuración del PWM_0, 3 estados: (10,20,15), empezando a nivel alto:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&gt;&gt; Misma instrucciones que la segunda parte del Test 11.3 hasta la actualización
+wait clk_period
+&gt;&gt; REG_CONTROL(0x04) = 0x00000004
+wait 1 min
+</t>
+    </r>
+  </si>
+  <si>
+    <t>El "update anticipado" no tiene efecto. Se aplica la primera configuración y después la siguiente. Funcionamiento normal.</t>
+  </si>
+  <si>
+    <t>1. No entra configuración porque salta error: las wr_addr del test anterior no se han reseteado y config_error no resetea la cuenta.</t>
+  </si>
+  <si>
+    <t>Pulso activo en la señal de reset tras configuraciones (una correcta y otra errónea).</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Primera configuración del PWM_0, 4 estados: (1,5,3,1), empezando a nivel alto:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+&gt;&gt; Mismas instrucciones que el Test 1 hasta el apagado
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Segunda configuración del PWM_0, 3 estados: (10,20,15), empezando a nivel alto:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+&gt;&gt; REG_DIRECCIONES(0x00) = 0x00000001
 &gt;&gt; REG_CONTROL(0x04) = 0x00000008
 &gt;&gt; REG_N_ADDR(0x10) = 0x00000003
 &gt;&gt; REG_N_TOT_CYC(0x14) = 0x0000002D
 &gt;&gt; REG_PWM_INIT(0x18) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x0000000A
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x00000014
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
 &gt;&gt; REG_WR_DATA(0x08) = 0x0000000F
-&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0X00000001
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
 &gt;&gt; REG_CONTROL(0x04) = 0x00000004
-wait 1 min</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Primera configuración del PWM_0, 4 estados: (1,5,3,1), empezando nivel alto:
-&gt;&gt; Mismas instrucciones que el Test 1 hasta el apagado
-Segunda configuración del PWM_0, 3 estados: (10,20,15), empezando nivel alto:
-&gt;&gt; Misma instrucciones que la segunda parte del Test 11.3 hasta la actualización
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-wait 2 clk_period
+wait clk_period
 &gt;&gt; REG_CONTROL(0x04) = 0x00000004
 wait 1 min
 </t>
     </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Apagado:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+&gt;&gt; REG_DIRECCIONES(0x00) = 0x00000001
+&gt;&gt; REG_CONTROL(0x04) = 0x00000002</t>
+    </r>
+  </si>
+  <si>
+    <t>0: - 
+1: Selec.</t>
+  </si>
+  <si>
+    <t>0: -
+1: Aplicar</t>
+  </si>
+  <si>
+    <t>0: -
+1: Enable</t>
+  </si>
+  <si>
+    <t>0: OK
+1: Error</t>
+  </si>
+  <si>
+    <t>000: Apagados
+001: Apagando
+010: Configurando
+011: Activos
+100: Error</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Todos apagados</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ninguno activo y al menos 1 apagándose</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Configurando
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Al menos 1 activo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Error</t>
+    </r>
+  </si>
+  <si>
+    <t>Se aplica la primera configuración todo el rato. La segunda configuración se pierde ya que el IP está protegido ante este caso. Salta error.</t>
+  </si>
+  <si>
+    <t>1. Se resetea el contador de wr_data en CONTROL_UNIT tras cada intento de actualización.</t>
+  </si>
+  <si>
+    <t>Se aplican ambas configuraciones de forma normal. El doble "update" no te efecto, pues el delay en las transacciones AXI escribe sobre el registro de control después del último dato.</t>
+  </si>
+  <si>
+    <t>1. No entra la segunda configuración correctamente.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Configuración del PWM_0, 4 estados: (1,5,3,1), empezando a nivel alto:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+&gt;&gt; Mismas instrucciones que el Test 1.1 hasta el apagado
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Configuración del PWM_0, 5 estados: (1,1,10,4,1), empezando a nivel bajo:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&gt;&gt; REG_DIRECCIONES(0x00 = 0x00000001
+&gt;&gt; REG_CONTROL(0x04) = 0x00000008
+&gt;&gt; REG_N_ADDR(0x10) = 0x00000005
+&gt;&gt; REG_N_TOT_CYC(0x14) = 0x000000011
+&gt;&gt; REG_PWM_INIT(0x18) = 0x00000000
+&gt;&gt; REG_WR_DATA(0x08) = 0x00000001
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
+&gt;&gt; REG_WR_DATA(0x08) = 0x00000001
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
+&gt;&gt; REG_WR_DATA(0x08) = 0x0000000A
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
+&gt;&gt; REG_WR_DATA(0x08) = 0x00000004
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
+&gt;&gt; REG_WR_DATA(0x08) = 0x00000001
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
+wait clk_period
+&gt;&gt; REG_CONTROL(0x04) = 0x00000004
+wait 1 min
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Configuración del PWM_0, 3 estados: (10,20,15), empezando a nivel alto:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&gt;&gt; REG_DIRECCIONES(0x00) = 0x00000001
+&gt;&gt; REG_CONTROL(0x04) = 0x00000008
+&gt;&gt; REG_N_ADDR(0x10) = 0x00000003
+&gt;&gt; REG_N_TOT_CYC(0x14) = 0x0000002D
+&gt;&gt; REG_PWM_INIT(0x18) = 0x00000001
+&gt;&gt; REG_WR_DATA(0x08) = 0x0000000A
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
+&gt;&gt; REG_WR_DATA(0x08) = 0x00000014
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
+&gt;&gt; REG_WR_DATA(0x08) = 0x0000000F
+&gt;&gt; REG_WR_DATA_VALID(0x0C) = 0x00000001
+wait clk_period
+&gt;&gt; REG_CONTROL(0x04) = 0x00000004
+wait 1 min
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Apagado:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+&gt;&gt; REG_DIRECCIONES(0x00) = 0x00000001
+&gt;&gt; REG_CONTROL(0x04) = 0x00000002</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Configuración del PWM_0, 4 estados: (1,5,3,1), empezando a nivel alto:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+&gt;&gt; Mismas instrucciones que el Test 1 hasta el apagado
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Reset:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+reset = '1'
+Segunda configuración del PWM_0, 3 estados: (10,20,15), empezando a nivel alto:
+&gt;&gt; Misma instrucciones que la segunda parte del Test 11.3 hasta la actualización</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Se usa early_sw para controlar la siguiente configuración en caso de no haber actualizado la anterior.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1345,6 +1953,34 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1418,7 +2054,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -1884,13 +2520,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1971,9 +2644,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
@@ -2036,9 +2706,6 @@
     <xf numFmtId="49" fontId="0" fillId="9" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2051,6 +2718,51 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2090,31 +2802,94 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2125,39 +2900,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2463,36 +3205,36 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:V34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
+      <pane ySplit="9" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.54296875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="20.7265625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.7265625" style="48" customWidth="1"/>
     <col min="3" max="3" width="45.6328125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="60.6328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="80.6328125" style="2" customWidth="1"/>
     <col min="5" max="5" width="30.7265625" style="2" customWidth="1"/>
     <col min="6" max="8" width="4.54296875" style="5" customWidth="1"/>
-    <col min="9" max="10" width="45.6328125" style="50" customWidth="1"/>
+    <col min="9" max="10" width="45.6328125" style="48" customWidth="1"/>
     <col min="11" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="58"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="71"/>
     </row>
     <row r="2" spans="1:10" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="11"/>
@@ -2571,39 +3313,39 @@
       <c r="H7" s="12"/>
     </row>
     <row r="8" spans="1:10" s="3" customFormat="1" ht="14.5" customHeight="1" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="65" t="s">
+      <c r="A8" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="63" t="s">
+      <c r="C8" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="63" t="s">
+      <c r="D8" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="63" t="s">
+      <c r="E8" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="59" t="s">
+      <c r="F8" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="59"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="54" t="s">
-        <v>134</v>
-      </c>
-      <c r="J8" s="88" t="s">
-        <v>174</v>
+      <c r="G8" s="72"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="67" t="s">
+        <v>124</v>
+      </c>
+      <c r="J8" s="65" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="66"/>
-      <c r="B9" s="64"/>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
+      <c r="A9" s="79"/>
+      <c r="B9" s="77"/>
+      <c r="C9" s="77"/>
+      <c r="D9" s="77"/>
+      <c r="E9" s="77"/>
       <c r="F9" s="4" t="s">
         <v>5</v>
       </c>
@@ -2613,422 +3355,537 @@
       <c r="H9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="55"/>
-      <c r="J9" s="89"/>
-    </row>
-    <row r="10" spans="1:10" customFormat="1" ht="275.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="14">
-        <v>1</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>56</v>
+      <c r="I9" s="68"/>
+      <c r="J9" s="66"/>
+    </row>
+    <row r="10" spans="1:10" customFormat="1" ht="304.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="B10" s="82" t="s">
+        <v>55</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="7" t="s">
+        <v>149</v>
+      </c>
       <c r="G10" s="7"/>
       <c r="H10" s="15"/>
-      <c r="I10" s="86" t="s">
-        <v>150</v>
-      </c>
-      <c r="J10" s="51" t="s">
+      <c r="I10" s="53" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" customFormat="1" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="16">
+      <c r="J10" s="49" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="87" t="s">
+        <v>146</v>
+      </c>
+      <c r="B11" s="86"/>
+      <c r="C11" s="82" t="s">
+        <v>148</v>
+      </c>
+      <c r="D11" s="82" t="s">
+        <v>193</v>
+      </c>
+      <c r="E11" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="93" t="s">
+        <v>149</v>
+      </c>
+      <c r="G11" s="93"/>
+      <c r="H11" s="91"/>
+      <c r="I11" s="89"/>
+      <c r="J11" s="84"/>
+    </row>
+    <row r="12" spans="1:10" customFormat="1" ht="224" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="88"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="83"/>
+      <c r="E12" s="94"/>
+      <c r="F12" s="94"/>
+      <c r="G12" s="94"/>
+      <c r="H12" s="92"/>
+      <c r="I12" s="90"/>
+      <c r="J12" s="85"/>
+    </row>
+    <row r="13" spans="1:10" customFormat="1" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="16">
         <v>2</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B13" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="51"/>
-    </row>
-    <row r="12" spans="1:10" customFormat="1" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="14">
-        <v>3</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>164</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="51"/>
-    </row>
-    <row r="13" spans="1:10" customFormat="1" ht="232" x14ac:dyDescent="0.35">
-      <c r="A13" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>18</v>
-      </c>
       <c r="C13" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="D13" s="87" t="s">
-        <v>165</v>
+        <v>140</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>161</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="9"/>
+      <c r="F13" s="9" t="s">
+        <v>149</v>
+      </c>
       <c r="G13" s="9"/>
       <c r="H13" s="17"/>
-      <c r="I13" s="86" t="s">
-        <v>152</v>
-      </c>
-      <c r="J13" s="86" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="33" customFormat="1" ht="232" x14ac:dyDescent="0.35">
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+    </row>
+    <row r="14" spans="1:10" customFormat="1" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A14" s="14">
-        <v>5</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>159</v>
+        <v>3</v>
+      </c>
+      <c r="B14" s="56" t="s">
+        <v>17</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>166</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="7"/>
+        <v>162</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>149</v>
+      </c>
       <c r="G14" s="7"/>
       <c r="H14" s="15"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="51"/>
-    </row>
-    <row r="15" spans="1:10" customFormat="1" ht="232" x14ac:dyDescent="0.35">
-      <c r="A15" s="16">
-        <v>6</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>19</v>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+    </row>
+    <row r="15" spans="1:10" customFormat="1" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="B15" s="80" t="s">
+        <v>18</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="E15" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="D15" s="54" t="s">
+        <v>163</v>
+      </c>
+      <c r="E15" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="9"/>
+      <c r="F15" s="9" t="s">
+        <v>149</v>
+      </c>
       <c r="G15" s="9"/>
       <c r="H15" s="17"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="51"/>
-    </row>
-    <row r="16" spans="1:10" customFormat="1" ht="333.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="14">
+      <c r="I15" s="53" t="s">
+        <v>152</v>
+      </c>
+      <c r="J15" s="53" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" customFormat="1" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="B16" s="81"/>
+      <c r="C16" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D16" s="54" t="s">
+        <v>164</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="53"/>
+    </row>
+    <row r="17" spans="1:22" s="32" customFormat="1" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="14">
+        <v>5</v>
+      </c>
+      <c r="B17" s="56" t="s">
+        <v>142</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G17" s="7"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="50"/>
+      <c r="P17"/>
+      <c r="V17"/>
+    </row>
+    <row r="18" spans="1:22" customFormat="1" ht="261" x14ac:dyDescent="0.35">
+      <c r="A18" s="16">
+        <v>6</v>
+      </c>
+      <c r="B18" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="E18" s="61" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="G18" s="9"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="49" t="s">
+        <v>168</v>
+      </c>
+      <c r="J18" s="49" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" customFormat="1" ht="348" x14ac:dyDescent="0.35">
+      <c r="A19" s="14">
         <v>7</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B19" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C19" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="51"/>
-      <c r="J16" s="51"/>
-    </row>
-    <row r="17" spans="1:10" customFormat="1" ht="290" x14ac:dyDescent="0.35">
-      <c r="A17" s="16">
-        <v>8</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
-    </row>
-    <row r="18" spans="1:10" customFormat="1" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="61" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="19" t="s">
+      <c r="D19" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="E18" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
-    </row>
-    <row r="19" spans="1:10" customFormat="1" ht="275.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="61"/>
-      <c r="C19" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>171</v>
-      </c>
       <c r="E19" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="F19" s="7"/>
+        <v>45</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>149</v>
+      </c>
       <c r="G19" s="7"/>
       <c r="H19" s="15"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="51"/>
-    </row>
-    <row r="20" spans="1:10" customFormat="1" ht="232" x14ac:dyDescent="0.35">
-      <c r="A20" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="62" t="s">
-        <v>26</v>
+      <c r="I19" s="49"/>
+      <c r="J19" s="49"/>
+    </row>
+    <row r="20" spans="1:22" customFormat="1" ht="304.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="16">
+        <v>8</v>
+      </c>
+      <c r="B20" s="57" t="s">
+        <v>21</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F20" s="9"/>
+        <v>171</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>149</v>
+      </c>
       <c r="G20" s="9"/>
       <c r="H20" s="17"/>
-      <c r="I20" s="51"/>
-      <c r="J20" s="51"/>
-    </row>
-    <row r="21" spans="1:10" customFormat="1" ht="232" x14ac:dyDescent="0.35">
-      <c r="A21" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="62"/>
-      <c r="C21" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="18" t="s">
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+    </row>
+    <row r="21" spans="1:22" customFormat="1" ht="203" x14ac:dyDescent="0.35">
+      <c r="A21" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="74" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G21" s="7"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="49"/>
+    </row>
+    <row r="22" spans="1:22" customFormat="1" ht="261" x14ac:dyDescent="0.35">
+      <c r="A22" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="74"/>
+      <c r="C22" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="E21" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="51"/>
-      <c r="J21" s="51"/>
-    </row>
-    <row r="22" spans="1:10" customFormat="1" ht="333.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="61" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>176</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="F22" s="7"/>
+      <c r="E22" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>149</v>
+      </c>
       <c r="G22" s="7"/>
       <c r="H22" s="15"/>
-      <c r="I22" s="51"/>
-      <c r="J22" s="51"/>
-    </row>
-    <row r="23" spans="1:10" customFormat="1" ht="319" x14ac:dyDescent="0.35">
-      <c r="A23" s="14" t="s">
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
+    </row>
+    <row r="23" spans="1:22" customFormat="1" ht="232" x14ac:dyDescent="0.35">
+      <c r="A23" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="75" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="G23" s="9"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+    </row>
+    <row r="24" spans="1:22" customFormat="1" ht="232" x14ac:dyDescent="0.35">
+      <c r="A24" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="75"/>
+      <c r="C24" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="G24" s="9"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+    </row>
+    <row r="25" spans="1:22" customFormat="1" ht="362.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="74" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G25" s="7"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="49"/>
+    </row>
+    <row r="26" spans="1:22" customFormat="1" ht="348" x14ac:dyDescent="0.35">
+      <c r="A26" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="74"/>
+      <c r="C26" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G26" s="7"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
+    </row>
+    <row r="27" spans="1:22" customFormat="1" ht="333.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="61"/>
-      <c r="C23" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="51"/>
-      <c r="J23" s="51"/>
-    </row>
-    <row r="24" spans="1:10" customFormat="1" ht="275.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="61"/>
-      <c r="C24" s="19" t="s">
+      <c r="B27" s="74"/>
+      <c r="C27" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="E27" s="62" t="s">
+        <v>191</v>
+      </c>
+      <c r="F27" s="63" t="s">
+        <v>149</v>
+      </c>
+      <c r="G27" s="7"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="49" t="s">
+        <v>180</v>
+      </c>
+      <c r="J27" s="49" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" customFormat="1" ht="145" x14ac:dyDescent="0.35">
+      <c r="A28" s="16">
+        <v>12</v>
+      </c>
+      <c r="B28" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="G28" s="9"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="64" t="s">
+        <v>192</v>
+      </c>
+      <c r="J28" s="64" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A29" s="21">
+        <v>13</v>
+      </c>
+      <c r="B29" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="55" t="s">
+        <v>123</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
+    </row>
+    <row r="30" spans="1:22" customFormat="1" ht="116.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="25">
+        <v>14</v>
+      </c>
+      <c r="B30" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="D24" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="E24" s="49" t="s">
-        <v>133</v>
-      </c>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="51"/>
-      <c r="J24" s="51"/>
-    </row>
-    <row r="25" spans="1:10" customFormat="1" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="16">
-        <v>12</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="52"/>
-      <c r="J25" s="52"/>
-    </row>
-    <row r="26" spans="1:10" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A26" s="21">
-        <v>13</v>
-      </c>
-      <c r="B26" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="52"/>
-      <c r="J26" s="52"/>
-    </row>
-    <row r="27" spans="1:10" customFormat="1" ht="261.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="25">
-        <v>14</v>
-      </c>
-      <c r="B27" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="27" t="s">
-        <v>161</v>
-      </c>
-      <c r="E27" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="53"/>
-      <c r="J27" s="53"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="D31" s="20"/>
+      <c r="C30" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="D30" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="E30" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="G30" s="27"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D34" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="23">
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="E11:E12"/>
     <mergeCell ref="J8:J9"/>
     <mergeCell ref="I8:I9"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="F8:H8"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B21:B22"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="C11:C12"/>
   </mergeCells>
-  <conditionalFormatting sqref="F10:H1048576">
+  <conditionalFormatting sqref="F10:H11 F13:H1048576">
     <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="F">
       <formula>NOT(ISERROR(SEARCH("F",F10)))</formula>
     </cfRule>
@@ -3045,692 +3902,710 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FEE446F-32F7-473D-A3EC-DB53D909EC6D}">
   <dimension ref="B1:K37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView topLeftCell="F16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.7265625" customWidth="1"/>
-    <col min="2" max="2" width="20.7265625" style="30" customWidth="1"/>
-    <col min="3" max="4" width="10.7265625" style="30" customWidth="1"/>
-    <col min="5" max="5" width="7.7265625" style="30" customWidth="1"/>
-    <col min="6" max="6" width="15.7265625" style="30" customWidth="1"/>
-    <col min="7" max="7" width="7.7265625" style="30" customWidth="1"/>
-    <col min="8" max="8" width="70.7265625" style="31" customWidth="1"/>
-    <col min="9" max="9" width="17.7265625" style="31" customWidth="1"/>
-    <col min="10" max="10" width="7.7265625" style="30" customWidth="1"/>
-    <col min="11" max="11" width="60.7265625" style="32" customWidth="1"/>
+    <col min="2" max="2" width="20.7265625" style="29" customWidth="1"/>
+    <col min="3" max="4" width="10.7265625" style="29" customWidth="1"/>
+    <col min="5" max="5" width="7.7265625" style="29" customWidth="1"/>
+    <col min="6" max="6" width="15.7265625" style="29" customWidth="1"/>
+    <col min="7" max="7" width="7.7265625" style="29" customWidth="1"/>
+    <col min="8" max="8" width="70.7265625" style="30" customWidth="1"/>
+    <col min="9" max="9" width="17.7265625" style="30" customWidth="1"/>
+    <col min="10" max="10" width="7.7265625" style="29" customWidth="1"/>
+    <col min="11" max="11" width="60.7265625" style="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:11" s="33" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="45" t="s">
+    <row r="2" spans="2:11" s="32" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="45" t="s">
-        <v>135</v>
-      </c>
-      <c r="D2" s="45" t="s">
-        <v>136</v>
-      </c>
-      <c r="E2" s="45" t="s">
+      <c r="H2" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="45" t="s">
+      <c r="J2" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" s="45" t="s">
         <v>61</v>
-      </c>
-      <c r="H2" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="J2" s="45" t="s">
-        <v>54</v>
-      </c>
-      <c r="K2" s="46" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="2:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="95" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="97" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="D4" s="97" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="70" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" s="34" t="s">
+      <c r="H4" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" s="34" t="s">
+        <v>183</v>
+      </c>
+      <c r="J4" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="K4" s="99" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="101"/>
+      <c r="C5" s="102"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="J5" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K5" s="103"/>
+    </row>
+    <row r="6" spans="2:11" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="96"/>
+      <c r="C6" s="98"/>
+      <c r="D6" s="98"/>
+      <c r="E6" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="H4" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="I4" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="J4" s="34" t="s">
+      <c r="H6" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" s="34" t="s">
+        <v>183</v>
+      </c>
+      <c r="J6" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="K6" s="100"/>
+    </row>
+    <row r="7" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="8" spans="2:11" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="95" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="97" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="97" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="K4" s="73" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B5" s="68"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="F5" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="G5" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="H5" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="I5" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="J5" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="K5" s="74"/>
-    </row>
-    <row r="6" spans="2:11" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="69"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="F6" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="G6" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="H6" s="39" t="s">
+      <c r="H8" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="I6" s="39" t="s">
-        <v>70</v>
-      </c>
-      <c r="J6" s="38" t="s">
+      <c r="I8" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="J8" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="K8" s="99" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="110"/>
+      <c r="C9" s="111"/>
+      <c r="D9" s="111"/>
+      <c r="E9" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="K6" s="75"/>
-    </row>
-    <row r="7" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="8" spans="2:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="B8" s="67" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="70" t="s">
+      <c r="H9" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="I9" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="J9" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="K9" s="112"/>
+    </row>
+    <row r="10" spans="2:11" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="110"/>
+      <c r="C10" s="111"/>
+      <c r="D10" s="111"/>
+      <c r="E10" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="70" t="s">
-        <v>104</v>
-      </c>
-      <c r="E8" s="34" t="s">
+      <c r="G10" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="F8" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="G8" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="H8" s="35" t="s">
-        <v>79</v>
-      </c>
-      <c r="I8" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="J8" s="34" t="s">
+      <c r="H10" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="I10" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="J10" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="K10" s="112"/>
+    </row>
+    <row r="11" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="B11" s="101"/>
+      <c r="C11" s="102"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="K8" s="73" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="B9" s="76"/>
-      <c r="C9" s="77"/>
-      <c r="D9" s="77"/>
-      <c r="E9" s="40" t="s">
-        <v>82</v>
-      </c>
-      <c r="F9" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="G9" s="40" t="s">
-        <v>68</v>
-      </c>
-      <c r="H9" s="41" t="s">
-        <v>84</v>
-      </c>
-      <c r="I9" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="J9" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="K9" s="78"/>
-    </row>
-    <row r="10" spans="2:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="B10" s="76"/>
-      <c r="C10" s="77"/>
-      <c r="D10" s="77"/>
-      <c r="E10" s="40" t="s">
-        <v>85</v>
-      </c>
-      <c r="F10" s="40" t="s">
+      <c r="H11" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="G10" s="40" t="s">
-        <v>68</v>
-      </c>
-      <c r="H10" s="41" t="s">
+      <c r="I11" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="J11" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="K11" s="103"/>
+    </row>
+    <row r="12" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="96"/>
+      <c r="C12" s="98"/>
+      <c r="D12" s="98"/>
+      <c r="E12" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="I10" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="J10" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="K10" s="78"/>
-    </row>
-    <row r="11" spans="2:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="B11" s="68"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="36" t="s">
+      <c r="F12" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="F11" s="36" t="s">
+      <c r="G12" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="G11" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="H11" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="I11" s="37" t="s">
-        <v>80</v>
-      </c>
-      <c r="J11" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="K11" s="74"/>
-    </row>
-    <row r="12" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="69"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="F12" s="38" t="s">
-        <v>92</v>
-      </c>
-      <c r="G12" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="H12" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="I12" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="J12" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="K12" s="75"/>
+      <c r="H12" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="I12" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="J12" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="K12" s="100"/>
     </row>
     <row r="13" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="14" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="47" t="s">
-        <v>94</v>
-      </c>
-      <c r="C14" s="48" t="s">
-        <v>85</v>
-      </c>
-      <c r="D14" s="48" t="s">
-        <v>119</v>
-      </c>
-      <c r="E14" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="F14" s="42" t="s">
-        <v>94</v>
-      </c>
-      <c r="G14" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="H14" s="43" t="s">
-        <v>96</v>
-      </c>
-      <c r="I14" s="43" t="s">
-        <v>97</v>
-      </c>
-      <c r="J14" s="42" t="s">
+      <c r="B14" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="G14" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="K14" s="44"/>
+      <c r="H14" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="I14" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="J14" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="K14" s="43"/>
     </row>
     <row r="15" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="16" spans="2:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="B16" s="79" t="s">
-        <v>98</v>
-      </c>
-      <c r="C16" s="81" t="s">
+      <c r="B16" s="104" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="106" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="106" t="s">
+        <v>127</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="G16" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="I16" s="34" t="s">
+        <v>185</v>
+      </c>
+      <c r="J16" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="K16" s="108" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="105"/>
+      <c r="C17" s="107"/>
+      <c r="D17" s="107"/>
+      <c r="E17" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="D16" s="81" t="s">
-        <v>137</v>
-      </c>
-      <c r="E16" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="F16" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="G16" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="H16" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I16" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="J16" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="K16" s="83" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="80"/>
-      <c r="C17" s="82"/>
-      <c r="D17" s="82"/>
-      <c r="E17" s="38" t="s">
-        <v>102</v>
-      </c>
-      <c r="F17" s="38" t="s">
-        <v>92</v>
-      </c>
-      <c r="G17" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="H17" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="I17" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="J17" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="K17" s="84"/>
+      <c r="G17" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="I17" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="J17" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="K17" s="109"/>
     </row>
     <row r="18" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="19" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="47" t="s">
-        <v>103</v>
-      </c>
-      <c r="C19" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="D19" s="48" t="s">
-        <v>144</v>
-      </c>
-      <c r="E19" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="F19" s="42" t="s">
-        <v>103</v>
-      </c>
-      <c r="G19" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="H19" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="I19" s="43" t="s">
-        <v>97</v>
-      </c>
-      <c r="J19" s="42" t="s">
+      <c r="B19" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="47" t="s">
+        <v>128</v>
+      </c>
+      <c r="D19" s="47" t="s">
+        <v>134</v>
+      </c>
+      <c r="E19" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="F19" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="G19" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="K19" s="44"/>
+      <c r="H19" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="I19" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="J19" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="K19" s="43"/>
     </row>
     <row r="20" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="21" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="47" t="s">
-        <v>106</v>
-      </c>
-      <c r="C21" s="48" t="s">
-        <v>139</v>
-      </c>
-      <c r="D21" s="48" t="s">
-        <v>145</v>
-      </c>
-      <c r="E21" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="F21" s="42" t="s">
-        <v>106</v>
-      </c>
-      <c r="G21" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="H21" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="I21" s="43" t="s">
-        <v>97</v>
-      </c>
-      <c r="J21" s="42" t="s">
+      <c r="B21" s="46" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="D21" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="G21" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="K21" s="44"/>
+      <c r="H21" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="I21" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="J21" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="K21" s="43"/>
     </row>
     <row r="22" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="23" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B23" s="67" t="s">
-        <v>108</v>
-      </c>
-      <c r="C23" s="70" t="s">
-        <v>140</v>
-      </c>
-      <c r="D23" s="70" t="s">
-        <v>146</v>
-      </c>
-      <c r="E23" s="34" t="s">
+      <c r="B23" s="95" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="97" t="s">
+        <v>130</v>
+      </c>
+      <c r="D23" s="97" t="s">
+        <v>136</v>
+      </c>
+      <c r="E23" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="G23" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="F23" s="34" t="s">
-        <v>109</v>
-      </c>
-      <c r="G23" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="H23" s="35" t="s">
-        <v>110</v>
-      </c>
-      <c r="I23" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="J23" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="K23" s="73"/>
+      <c r="H23" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="I23" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="J23" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="K23" s="99"/>
     </row>
     <row r="24" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="69"/>
-      <c r="C24" s="72"/>
-      <c r="D24" s="72"/>
-      <c r="E24" s="38" t="s">
-        <v>102</v>
-      </c>
-      <c r="F24" s="38" t="s">
-        <v>92</v>
-      </c>
-      <c r="G24" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="H24" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="I24" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="J24" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="K24" s="75"/>
+      <c r="B24" s="96"/>
+      <c r="C24" s="98"/>
+      <c r="D24" s="98"/>
+      <c r="E24" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="F24" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="G24" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="H24" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="I24" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="J24" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="K24" s="100"/>
     </row>
     <row r="25" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="26" spans="2:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="B26" s="67" t="s">
+      <c r="B26" s="95" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="97" t="s">
+        <v>131</v>
+      </c>
+      <c r="D26" s="97" t="s">
+        <v>137</v>
+      </c>
+      <c r="E26" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="G26" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="H26" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="I26" s="34" t="s">
+        <v>186</v>
+      </c>
+      <c r="J26" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="K26" s="99"/>
+    </row>
+    <row r="27" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="101"/>
+      <c r="C27" s="102"/>
+      <c r="D27" s="102"/>
+      <c r="E27" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="G27" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="H27" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="I27" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="J27" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K27" s="103"/>
+    </row>
+    <row r="28" spans="2:11" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B28" s="96"/>
+      <c r="C28" s="98"/>
+      <c r="D28" s="98"/>
+      <c r="E28" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F28" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="G28" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="H28" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="C26" s="70" t="s">
-        <v>141</v>
-      </c>
-      <c r="D26" s="70" t="s">
-        <v>147</v>
-      </c>
-      <c r="E26" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="F26" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="G26" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="H26" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="I26" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="J26" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="K26" s="73"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B27" s="68"/>
-      <c r="C27" s="71"/>
-      <c r="D27" s="71"/>
-      <c r="E27" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="F27" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="G27" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="H27" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="I27" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="J27" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="K27" s="74"/>
-    </row>
-    <row r="28" spans="2:11" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="69"/>
-      <c r="C28" s="72"/>
-      <c r="D28" s="72"/>
-      <c r="E28" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="F28" s="38" t="s">
-        <v>116</v>
-      </c>
-      <c r="G28" s="38" t="s">
-        <v>113</v>
-      </c>
-      <c r="H28" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="I28" s="39" t="s">
-        <v>115</v>
-      </c>
-      <c r="J28" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="K28" s="75"/>
+      <c r="I28" s="34" t="s">
+        <v>186</v>
+      </c>
+      <c r="J28" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="K28" s="100"/>
     </row>
     <row r="29" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="30" spans="2:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="B30" s="67" t="s">
+      <c r="B30" s="95" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" s="97" t="s">
+        <v>132</v>
+      </c>
+      <c r="D30" s="97" t="s">
+        <v>138</v>
+      </c>
+      <c r="E30" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="F30" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="G30" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="H30" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="I30" s="34" t="s">
+        <v>186</v>
+      </c>
+      <c r="J30" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="K30" s="99" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B31" s="101"/>
+      <c r="C31" s="102"/>
+      <c r="D31" s="102"/>
+      <c r="E31" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="F31" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="G31" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="H31" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="I31" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="J31" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K31" s="103"/>
+    </row>
+    <row r="32" spans="2:11" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="96"/>
+      <c r="C32" s="98"/>
+      <c r="D32" s="98"/>
+      <c r="E32" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="G32" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="H32" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="C30" s="70" t="s">
-        <v>142</v>
-      </c>
-      <c r="D30" s="70" t="s">
-        <v>148</v>
-      </c>
-      <c r="E30" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="F30" s="34" t="s">
+      <c r="I32" s="34" t="s">
+        <v>186</v>
+      </c>
+      <c r="J32" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="K32" s="100"/>
+    </row>
+    <row r="33" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="34" spans="2:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B34" s="95" t="s">
+        <v>119</v>
+      </c>
+      <c r="C34" s="97" t="s">
+        <v>133</v>
+      </c>
+      <c r="D34" s="97" t="s">
+        <v>139</v>
+      </c>
+      <c r="E34" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="G30" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="H30" s="35" t="s">
+      <c r="F34" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="G34" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="H34" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="I30" s="35" t="s">
+      <c r="I34" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="J34" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="K34" s="99" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B35" s="96"/>
+      <c r="C35" s="98"/>
+      <c r="D35" s="98"/>
+      <c r="E35" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="J30" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="K30" s="73" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B31" s="68"/>
-      <c r="C31" s="71"/>
-      <c r="D31" s="71"/>
-      <c r="E31" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="F31" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="G31" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="H31" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="I31" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="J31" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="K31" s="74"/>
-    </row>
-    <row r="32" spans="2:11" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="69"/>
-      <c r="C32" s="72"/>
-      <c r="D32" s="72"/>
-      <c r="E32" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="F32" s="38" t="s">
-        <v>124</v>
-      </c>
-      <c r="G32" s="38" t="s">
-        <v>113</v>
-      </c>
-      <c r="H32" s="39" t="s">
-        <v>125</v>
-      </c>
-      <c r="I32" s="39" t="s">
-        <v>122</v>
-      </c>
-      <c r="J32" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="K32" s="75"/>
-    </row>
-    <row r="33" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="34" spans="2:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="B34" s="67" t="s">
-        <v>126</v>
-      </c>
-      <c r="C34" s="70" t="s">
-        <v>143</v>
-      </c>
-      <c r="D34" s="70" t="s">
-        <v>149</v>
-      </c>
-      <c r="E34" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="F34" s="34" t="s">
-        <v>126</v>
-      </c>
-      <c r="G34" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="H34" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="I34" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="J34" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="K34" s="73"/>
-    </row>
-    <row r="35" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="69"/>
-      <c r="C35" s="72"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="38" t="s">
-        <v>130</v>
-      </c>
-      <c r="F35" s="38" t="s">
-        <v>92</v>
-      </c>
-      <c r="G35" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="H35" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="I35" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="J35" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="K35" s="75"/>
+      <c r="F35" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="G35" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="H35" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="I35" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="J35" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="K35" s="100"/>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="D37" s="85"/>
+      <c r="D37" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="K4:K6"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="D8:D12"/>
+    <mergeCell ref="K8:K12"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C23:C24"/>
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="D34:D35"/>
     <mergeCell ref="K34:K35"/>
@@ -3743,23 +4618,8 @@
     <mergeCell ref="C26:C28"/>
     <mergeCell ref="C30:C32"/>
     <mergeCell ref="C34:C35"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="K4:K6"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="D8:D12"/>
-    <mergeCell ref="K8:K12"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="C8:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>